<commit_message>
implemented several GET requests
</commit_message>
<xml_diff>
--- a/SOA/SOA_PROJEKAT_1/SOA_PROJEKAT_1/Sensor_Device_Service/Data/SOA_DATA.xlsx
+++ b/SOA/SOA_PROJEKAT_1/SOA_PROJEKAT_1/Sensor_Device_Service/Data/SOA_DATA.xlsx
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,6 +432,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1451625299</v>
+      </c>
       <c r="B1">
         <v>1.2</v>
       </c>

</xml_diff>